<commit_message>
ornek gider dosyasi yenilendi
</commit_message>
<xml_diff>
--- a/etikom/static/file/ornek-gider-dosyasi.xlsx
+++ b/etikom/static/file/ornek-gider-dosyasi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oktay\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186263AB-CA80-42BE-8D56-8BD4269694D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD54AA7F-10B3-44A7-A647-419A575B61D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>Başlık</t>
   </si>
@@ -34,28 +34,16 @@
     <t>Ambalaj Gideri</t>
   </si>
   <si>
-    <t>19.05.2024</t>
-  </si>
-  <si>
     <t>Ceza Gideri</t>
   </si>
   <si>
-    <t>11.05.2024</t>
-  </si>
-  <si>
     <t>Kira Gideri</t>
   </si>
   <si>
     <t>Reklam Gideri</t>
   </si>
   <si>
-    <t>23.03.2024</t>
-  </si>
-  <si>
     <t>Patpat Gideri</t>
-  </si>
-  <si>
-    <t>07.01.2024</t>
   </si>
 </sst>
 </file>
@@ -128,7 +116,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -139,15 +127,10 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +436,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.47265625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -473,10 +458,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>45374</v>
       </c>
       <c r="C2" s="3">
         <v>2450</v>
@@ -486,8 +471,8 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
+      <c r="B3" s="5">
+        <v>45431</v>
       </c>
       <c r="C3" s="3">
         <v>8450</v>
@@ -495,10 +480,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="5">
+        <v>45423</v>
       </c>
       <c r="C4" s="3">
         <v>75</v>
@@ -508,8 +493,8 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
+      <c r="B5" s="5">
+        <v>45298</v>
       </c>
       <c r="C5" s="3">
         <v>8300</v>
@@ -517,12 +502,12 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>45528</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>5200</v>
       </c>
     </row>
@@ -533,35 +518,35 @@
       <c r="B7" s="5">
         <v>45486</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>9000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="5">
         <v>45467</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="5">
         <v>45464</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>2050</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5">
         <v>45424</v>
@@ -572,7 +557,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" s="5">
         <v>45383</v>
@@ -588,13 +573,13 @@
       <c r="B12" s="5">
         <v>45373</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>8300</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" s="5">
         <v>45352</v>
@@ -605,18 +590,18 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B14" s="5">
         <v>45331</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>2400</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15" s="5">
         <v>45323</v>
@@ -627,18 +612,18 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16" s="5">
         <v>45305</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <v>1800</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B17" s="5">
         <v>45292</v>

</xml_diff>